<commit_message>
update bi import Nov 10
</commit_message>
<xml_diff>
--- a/bi_generic_import/Sample XLS-CSV File/Sample XLS File/product_variant.xlsx
+++ b/bi_generic_import/Sample XLS-CSV File/Sample XLS File/product_variant.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="68">
   <si>
     <t xml:space="preserve">NAME</t>
   </si>
@@ -97,6 +97,27 @@
     <t xml:space="preserve">x_bool</t>
   </si>
   <si>
+    <t xml:space="preserve">Attribute</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Variant Value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Variant price (Value Price Extra)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">analytic_account_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Expense Account (property_account_Expense_id)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Income Account (property_account_Income_id)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Routes (Route_ids)</t>
+  </si>
+  <si>
     <t xml:space="preserve">monitor</t>
   </si>
   <si>
@@ -109,7 +130,7 @@
     <t xml:space="preserve">Stockable Product</t>
   </si>
   <si>
-    <t xml:space="preserve">345566</t>
+    <t xml:space="preserve">34556f65</t>
   </si>
   <si>
     <t xml:space="preserve">Units</t>
@@ -130,25 +151,43 @@
     <t xml:space="preserve">red</t>
   </si>
   <si>
+    <t xml:space="preserve">Color</t>
+  </si>
+  <si>
+    <t xml:space="preserve">White</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Administrative</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Buy</t>
+  </si>
+  <si>
     <t xml:space="preserve">HP0013</t>
   </si>
   <si>
     <t xml:space="preserve">Internal</t>
   </si>
   <si>
-    <t xml:space="preserve">996776</t>
+    <t xml:space="preserve">99677f615</t>
   </si>
   <si>
     <t xml:space="preserve">blue</t>
   </si>
   <si>
+    <t xml:space="preserve">Black</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manufacture</t>
+  </si>
+  <si>
     <t xml:space="preserve">BOX</t>
   </si>
   <si>
     <t xml:space="preserve">ST0011</t>
   </si>
   <si>
-    <t xml:space="preserve">558585585</t>
+    <t xml:space="preserve">558585f5585</t>
   </si>
   <si>
     <t xml:space="preserve">https://ii1.pepperfry.com/media/catalog/product/s/o/494x544/solids-premium-canvas---mdf-15-litres-wardrobe-box--maroon---cream-solids-premium-canvas---mdf-15-li-e2dg4s.jpg</t>
@@ -160,6 +199,12 @@
     <t xml:space="preserve">purple</t>
   </si>
   <si>
+    <t xml:space="preserve">Legs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Steel</t>
+  </si>
+  <si>
     <t xml:space="preserve">Smart Phone</t>
   </si>
   <si>
@@ -169,13 +214,16 @@
     <t xml:space="preserve">Software</t>
   </si>
   <si>
-    <t xml:space="preserve">B1110001</t>
+    <t xml:space="preserve">B1110f0051</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.popsci.com/resizer/6iA2dK-qrizE_TrGloIM5mYz5Mw=/760x570/filters:focal(600x450:601x451)/arc-anglerfish-arc2-prod-bonnier.s3.amazonaws.com/public/VYHDQWEYQJMUBJTKNV4MMC5KMU.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">white</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Custom</t>
   </si>
 </sst>
 </file>
@@ -187,7 +235,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -214,18 +262,7 @@
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF0000FF"/>
-      <name val="Arial"/>
-      <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -270,7 +307,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -287,19 +324,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -324,25 +349,31 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Y6"/>
+  <dimension ref="A1:AF5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="N1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="T6" activeCellId="0" sqref="T6:Y6"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I13" activeCellId="0" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.39"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="15" min="5" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="53.63"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="18" min="17" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="19.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="25.14"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="21" style="0" width="11.52"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="15" min="5" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="49.2704081632653"/>
+    <col collapsed="false" hidden="false" max="18" min="17" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="22.8112244897959"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="27" min="22" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="25.1071428571429"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="31" min="30" style="0" width="37.3928571428571"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="1025" min="33" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -418,34 +449,55 @@
       <c r="Y1" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="Z1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD1" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE1" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF1" s="0" t="s">
+        <v>31</v>
+      </c>
     </row>
-    <row r="2" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="L2" s="1" t="n">
         <v>100</v>
@@ -459,53 +511,74 @@
       <c r="O2" s="1" t="n">
         <v>44</v>
       </c>
-      <c r="P2" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q2" s="5" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="R2" s="5" t="n">
+      <c r="P2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q2" s="4" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="R2" s="4" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="S2" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="T2" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="U2" s="6" t="s">
-        <v>34</v>
+      <c r="T2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="V2" s="1" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="W2" s="1" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="X2" s="1" t="n">
         <v>10000</v>
       </c>
-      <c r="Y2" s="7" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+      <c r="Y2" s="0" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="Z2" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA2" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB2" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="AC2" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="AD2" s="0" t="n">
+        <v>101401</v>
+      </c>
+      <c r="AE2" s="0" t="n">
+        <v>110100</v>
+      </c>
+      <c r="AF2" s="0" t="s">
+        <v>46</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="3" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
@@ -523,53 +596,74 @@
       <c r="O3" s="1" t="n">
         <v>32</v>
       </c>
-      <c r="P3" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q3" s="5" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="R3" s="8" t="n">
+      <c r="P3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q3" s="4" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="R3" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="S3" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="T3" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="U3" s="6" t="s">
-        <v>34</v>
+      <c r="T3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="V3" s="1" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="W3" s="1" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="X3" s="1" t="n">
         <v>50000</v>
       </c>
-      <c r="Y3" s="7" t="n">
+      <c r="Y3" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
+      <c r="Z3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA3" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="AB3" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="AC3" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="AD3" s="0" t="n">
+        <v>101401</v>
+      </c>
+      <c r="AE3" s="0" t="n">
+        <v>110100</v>
+      </c>
+      <c r="AF3" s="0" t="s">
+        <v>52</v>
+      </c>
     </row>
-    <row r="4" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="3" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
@@ -587,56 +681,77 @@
       <c r="O4" s="1" t="n">
         <v>32</v>
       </c>
-      <c r="P4" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q4" s="8" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="R4" s="8" t="n">
+      <c r="P4" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q4" s="5" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="R4" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="S4" s="1"/>
-      <c r="T4" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="U4" s="6" t="s">
-        <v>34</v>
+      <c r="T4" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="U4" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="V4" s="1" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="W4" s="1" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="X4" s="1" t="n">
         <v>100000</v>
       </c>
-      <c r="Y4" s="7" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+      <c r="Y4" s="0" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="Z4" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="AA4" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="AB4" s="0" t="n">
+        <v>300</v>
+      </c>
+      <c r="AC4" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="AD4" s="0" t="n">
+        <v>101401</v>
+      </c>
+      <c r="AE4" s="0" t="n">
+        <v>110100</v>
+      </c>
+      <c r="AF4" s="0" t="s">
+        <v>52</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="L5" s="0" t="n">
         <v>499</v>
@@ -650,41 +765,61 @@
       <c r="O5" s="0" t="n">
         <v>25</v>
       </c>
-      <c r="P5" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q5" s="8" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="R5" s="8" t="n">
+      <c r="P5" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q5" s="5" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="R5" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="S5" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="T5" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="U5" s="6" t="s">
-        <v>34</v>
+      <c r="T5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="U5" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="V5" s="1" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="W5" s="1" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="X5" s="1" t="n">
         <v>10000</v>
       </c>
-      <c r="Y5" s="7" t="n">
+      <c r="Y5" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
+      <c r="Z5" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AA5" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB5" s="0" t="n">
+        <v>400</v>
+      </c>
+      <c r="AC5" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="AD5" s="0" t="n">
+        <v>101401</v>
+      </c>
+      <c r="AE5" s="0" t="n">
+        <v>110100</v>
+      </c>
+      <c r="AF5" s="0" t="s">
+        <v>52</v>
+      </c>
     </row>
-    <row r="6" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="T1" r:id="rId1" display="x_partner_id@name"/>
@@ -696,7 +831,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
update bi import v Nov 10 dev
</commit_message>
<xml_diff>
--- a/bi_generic_import/Sample XLS-CSV File/Sample XLS File/product_variant.xlsx
+++ b/bi_generic_import/Sample XLS-CSV File/Sample XLS File/product_variant.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="68">
   <si>
     <t xml:space="preserve">NAME</t>
   </si>
@@ -97,6 +97,27 @@
     <t xml:space="preserve">x_bool</t>
   </si>
   <si>
+    <t xml:space="preserve">Attribute</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Variant Value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Variant price (Value Price Extra)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">analytic_account_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Expense Account (property_account_Expense_id)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Income Account (property_account_Income_id)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Routes (Route_ids)</t>
+  </si>
+  <si>
     <t xml:space="preserve">monitor</t>
   </si>
   <si>
@@ -109,7 +130,7 @@
     <t xml:space="preserve">Stockable Product</t>
   </si>
   <si>
-    <t xml:space="preserve">345566</t>
+    <t xml:space="preserve">34556f65</t>
   </si>
   <si>
     <t xml:space="preserve">Units</t>
@@ -130,25 +151,43 @@
     <t xml:space="preserve">red</t>
   </si>
   <si>
+    <t xml:space="preserve">Color</t>
+  </si>
+  <si>
+    <t xml:space="preserve">White</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Administrative</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Buy</t>
+  </si>
+  <si>
     <t xml:space="preserve">HP0013</t>
   </si>
   <si>
     <t xml:space="preserve">Internal</t>
   </si>
   <si>
-    <t xml:space="preserve">996776</t>
+    <t xml:space="preserve">99677f615</t>
   </si>
   <si>
     <t xml:space="preserve">blue</t>
   </si>
   <si>
+    <t xml:space="preserve">Black</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manufacture</t>
+  </si>
+  <si>
     <t xml:space="preserve">BOX</t>
   </si>
   <si>
     <t xml:space="preserve">ST0011</t>
   </si>
   <si>
-    <t xml:space="preserve">558585585</t>
+    <t xml:space="preserve">558585f5585</t>
   </si>
   <si>
     <t xml:space="preserve">https://ii1.pepperfry.com/media/catalog/product/s/o/494x544/solids-premium-canvas---mdf-15-litres-wardrobe-box--maroon---cream-solids-premium-canvas---mdf-15-li-e2dg4s.jpg</t>
@@ -160,6 +199,12 @@
     <t xml:space="preserve">purple</t>
   </si>
   <si>
+    <t xml:space="preserve">Legs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Steel</t>
+  </si>
+  <si>
     <t xml:space="preserve">Smart Phone</t>
   </si>
   <si>
@@ -169,13 +214,16 @@
     <t xml:space="preserve">Software</t>
   </si>
   <si>
-    <t xml:space="preserve">B1110001</t>
+    <t xml:space="preserve">B1110f0051</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.popsci.com/resizer/6iA2dK-qrizE_TrGloIM5mYz5Mw=/760x570/filters:focal(600x450:601x451)/arc-anglerfish-arc2-prod-bonnier.s3.amazonaws.com/public/VYHDQWEYQJMUBJTKNV4MMC5KMU.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">white</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Custom</t>
   </si>
 </sst>
 </file>
@@ -187,7 +235,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -214,18 +262,7 @@
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF0000FF"/>
-      <name val="Arial"/>
-      <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -270,7 +307,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -287,19 +324,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -324,25 +349,31 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Y6"/>
+  <dimension ref="A1:AF5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="N1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="T6" activeCellId="0" sqref="T6:Y6"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I13" activeCellId="0" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.39"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="15" min="5" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="53.63"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="18" min="17" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="19.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="25.14"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="21" style="0" width="11.52"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="15" min="5" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="49.2704081632653"/>
+    <col collapsed="false" hidden="false" max="18" min="17" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="22.8112244897959"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="27" min="22" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="25.1071428571429"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="31" min="30" style="0" width="37.3928571428571"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="1025" min="33" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -418,34 +449,55 @@
       <c r="Y1" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="Z1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD1" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE1" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF1" s="0" t="s">
+        <v>31</v>
+      </c>
     </row>
-    <row r="2" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="L2" s="1" t="n">
         <v>100</v>
@@ -459,53 +511,74 @@
       <c r="O2" s="1" t="n">
         <v>44</v>
       </c>
-      <c r="P2" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q2" s="5" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="R2" s="5" t="n">
+      <c r="P2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q2" s="4" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="R2" s="4" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="S2" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="T2" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="U2" s="6" t="s">
-        <v>34</v>
+      <c r="T2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="V2" s="1" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="W2" s="1" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="X2" s="1" t="n">
         <v>10000</v>
       </c>
-      <c r="Y2" s="7" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+      <c r="Y2" s="0" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="Z2" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA2" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB2" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="AC2" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="AD2" s="0" t="n">
+        <v>101401</v>
+      </c>
+      <c r="AE2" s="0" t="n">
+        <v>110100</v>
+      </c>
+      <c r="AF2" s="0" t="s">
+        <v>46</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="3" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
@@ -523,53 +596,74 @@
       <c r="O3" s="1" t="n">
         <v>32</v>
       </c>
-      <c r="P3" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q3" s="5" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="R3" s="8" t="n">
+      <c r="P3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q3" s="4" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="R3" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="S3" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="T3" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="U3" s="6" t="s">
-        <v>34</v>
+      <c r="T3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="V3" s="1" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="W3" s="1" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="X3" s="1" t="n">
         <v>50000</v>
       </c>
-      <c r="Y3" s="7" t="n">
+      <c r="Y3" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
+      <c r="Z3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA3" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="AB3" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="AC3" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="AD3" s="0" t="n">
+        <v>101401</v>
+      </c>
+      <c r="AE3" s="0" t="n">
+        <v>110100</v>
+      </c>
+      <c r="AF3" s="0" t="s">
+        <v>52</v>
+      </c>
     </row>
-    <row r="4" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="3" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
@@ -587,56 +681,77 @@
       <c r="O4" s="1" t="n">
         <v>32</v>
       </c>
-      <c r="P4" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q4" s="8" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="R4" s="8" t="n">
+      <c r="P4" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q4" s="5" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="R4" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="S4" s="1"/>
-      <c r="T4" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="U4" s="6" t="s">
-        <v>34</v>
+      <c r="T4" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="U4" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="V4" s="1" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="W4" s="1" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="X4" s="1" t="n">
         <v>100000</v>
       </c>
-      <c r="Y4" s="7" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+      <c r="Y4" s="0" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="Z4" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="AA4" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="AB4" s="0" t="n">
+        <v>300</v>
+      </c>
+      <c r="AC4" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="AD4" s="0" t="n">
+        <v>101401</v>
+      </c>
+      <c r="AE4" s="0" t="n">
+        <v>110100</v>
+      </c>
+      <c r="AF4" s="0" t="s">
+        <v>52</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="L5" s="0" t="n">
         <v>499</v>
@@ -650,41 +765,61 @@
       <c r="O5" s="0" t="n">
         <v>25</v>
       </c>
-      <c r="P5" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q5" s="8" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="R5" s="8" t="n">
+      <c r="P5" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q5" s="5" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="R5" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="S5" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="T5" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="U5" s="6" t="s">
-        <v>34</v>
+      <c r="T5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="U5" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="V5" s="1" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="W5" s="1" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="X5" s="1" t="n">
         <v>10000</v>
       </c>
-      <c r="Y5" s="7" t="n">
+      <c r="Y5" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
+      <c r="Z5" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AA5" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB5" s="0" t="n">
+        <v>400</v>
+      </c>
+      <c r="AC5" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="AD5" s="0" t="n">
+        <v>101401</v>
+      </c>
+      <c r="AE5" s="0" t="n">
+        <v>110100</v>
+      </c>
+      <c r="AF5" s="0" t="s">
+        <v>52</v>
+      </c>
     </row>
-    <row r="6" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="T1" r:id="rId1" display="x_partner_id@name"/>
@@ -696,7 +831,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>